<commit_message>
mise a jour dico des données
</commit_message>
<xml_diff>
--- a/1_Analyse/2_Dictionnaire des données/dico-des-donnees.xlsx
+++ b/1_Analyse/2_Dictionnaire des données/dico-des-donnees.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC-Olivier\Documents\GitHub\beaute-naturelle.fr\1_Analyse\2_Dictionnaire des données\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3FF15B-FC0B-4DAF-BEC0-C7124BA68FD7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486A429C-6BA1-487F-B8C9-036F407D190C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C1703559-1479-48AD-8C45-F5A1E66147F1}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
   <si>
     <t>Intitulé du champ</t>
   </si>
@@ -69,9 +69,6 @@
     <t>sexe</t>
   </si>
   <si>
-    <t>tel</t>
-  </si>
-  <si>
     <t>publier</t>
   </si>
   <si>
@@ -126,18 +123,6 @@
     <t>VARCHAR(30)</t>
   </si>
   <si>
-    <t xml:space="preserve">identifiant </t>
-  </si>
-  <si>
-    <t xml:space="preserve">pseudo </t>
-  </si>
-  <si>
-    <t xml:space="preserve">mot de passe </t>
-  </si>
-  <si>
-    <t xml:space="preserve">date inscription </t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -151,6 +136,51 @@
   </si>
   <si>
     <t>TEXT</t>
+  </si>
+  <si>
+    <t>date inscription de l'utilisateur</t>
+  </si>
+  <si>
+    <t>mot de passe de l'utilisateur</t>
+  </si>
+  <si>
+    <t>pseudo de l'utilisateur</t>
+  </si>
+  <si>
+    <t>nom de l'utilisateur</t>
+  </si>
+  <si>
+    <t>age de l'utilisateur</t>
+  </si>
+  <si>
+    <t>sexe de l'utilisateur</t>
+  </si>
+  <si>
+    <t>identifiant de l'utilisateur</t>
+  </si>
+  <si>
+    <t>prénom  de l'utilisateur</t>
+  </si>
+  <si>
+    <t>email  de l'utilisateur</t>
+  </si>
+  <si>
+    <t>téléhpone de l'utilisateur</t>
+  </si>
+  <si>
+    <t>adresse</t>
+  </si>
+  <si>
+    <t>cp</t>
+  </si>
+  <si>
+    <t>tel_fixe</t>
+  </si>
+  <si>
+    <t>tel_mobile</t>
+  </si>
+  <si>
+    <t>ville</t>
   </si>
 </sst>
 </file>
@@ -236,12 +266,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EF723056-E4B8-4061-80B1-0C4921BF2AB7}" name="Tableau2" displayName="Tableau2" ref="A1:C1048575" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EF723056-E4B8-4061-80B1-0C4921BF2AB7}" name="Tableau2" displayName="Tableau2" ref="A1:C1048575" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A1:C1048575" xr:uid="{369D7CF8-C4A2-4986-BDE3-A03DA8D931CC}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{94063425-DECB-4A76-A3E0-1A81E0A5F2CB}" name="Nom du champ" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{019612D5-0932-47FE-B3F8-53219A6E2896}" name="Type de données" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{066C183E-2CB4-4A03-95ED-B26B08FA63FF}" name="Intitulé du champ" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{94063425-DECB-4A76-A3E0-1A81E0A5F2CB}" name="Nom du champ" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{019612D5-0932-47FE-B3F8-53219A6E2896}" name="Type de données" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{066C183E-2CB4-4A03-95ED-B26B08FA63FF}" name="Intitulé du champ" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -544,17 +574,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DB9C3E5-8CF1-486C-8BD3-BBBC2F44537D}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" style="1" customWidth="1"/>
     <col min="4" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
@@ -571,7 +601,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -579,10 +609,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -590,10 +620,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -601,10 +631,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -612,10 +642,10 @@
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -623,7 +653,10 @@
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -631,7 +664,10 @@
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -639,7 +675,10 @@
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -647,137 +686,146 @@
         <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>3</v>
+      <c r="A13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>38</v>
+      <c r="A17" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>15</v>
+      <c r="A19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>26</v>
+      <c r="A23" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -785,7 +833,39 @@
         <v>20</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>24</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mis a jour dico des données
</commit_message>
<xml_diff>
--- a/1_Analyse/2_Dictionnaire des données/dico-des-donnees.xlsx
+++ b/1_Analyse/2_Dictionnaire des données/dico-des-donnees.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC-Olivier\Documents\GitHub\beaute-naturelle.fr\1_Analyse\2_Dictionnaire des données\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E06B21A-1885-4754-A548-1BA08F23B0BD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C05745-BC3C-47DF-B6E5-37DB16B43D7D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C1703559-1479-48AD-8C45-F5A1E66147F1}"/>
   </bookViews>
@@ -321,10 +321,10 @@
     <t xml:space="preserve"> identifiant du slide</t>
   </si>
   <si>
-    <t>source  de l'image de font du slide</t>
-  </si>
-  <si>
     <t>texte dans la bannière</t>
+  </si>
+  <si>
+    <t>source  de l'image de fond du slide</t>
   </si>
 </sst>
 </file>
@@ -718,10 +718,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DB9C3E5-8CF1-486C-8BD3-BBBC2F44537D}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1259,7 +1262,7 @@
         <v>25</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1270,12 +1273,12 @@
         <v>33</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="10" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>

<commit_message>
mise a jour et modification
</commit_message>
<xml_diff>
--- a/1_Analyse/2_Dictionnaire des données/dico-des-donnees.xlsx
+++ b/1_Analyse/2_Dictionnaire des données/dico-des-donnees.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\disiitp10\Documents\GitHub\beaute-naturelle.fr\1_Analyse\2_Dictionnaire des données\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC-Olivier\Documents\GitHub\beaute-naturelle.fr\1_Analyse\2_Dictionnaire des données\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F33C8B4-E529-4D8A-B086-590195F7E871}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC75459E-AA7D-4640-8D9E-D308F6B423FB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{C1703559-1479-48AD-8C45-F5A1E66147F1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C1703559-1479-48AD-8C45-F5A1E66147F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="139">
   <si>
     <t>Intitulé du champ</t>
   </si>
@@ -42,39 +42,6 @@
     <t>Type de données</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>nom</t>
-  </si>
-  <si>
-    <t>evenement</t>
-  </si>
-  <si>
-    <t>utilisateur</t>
-  </si>
-  <si>
-    <t>date_debut</t>
-  </si>
-  <si>
-    <t>date_fin</t>
-  </si>
-  <si>
-    <t>nbre_place_max</t>
-  </si>
-  <si>
-    <t>nbre_place_dispo</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>image</t>
-  </si>
-  <si>
-    <t>slug</t>
-  </si>
-  <si>
     <t>INT</t>
   </si>
   <si>
@@ -153,21 +120,6 @@
     <t>nombre de place maximum de l'événement</t>
   </si>
   <si>
-    <t>nombre de place disponible de l'événement</t>
-  </si>
-  <si>
-    <t>src</t>
-  </si>
-  <si>
-    <t>auteur</t>
-  </si>
-  <si>
-    <t>date_publi</t>
-  </si>
-  <si>
-    <t>libelle</t>
-  </si>
-  <si>
     <t>identifiant de l'image</t>
   </si>
   <si>
@@ -189,27 +141,6 @@
     <t>date de publication de l'image</t>
   </si>
   <si>
-    <t>galerie</t>
-  </si>
-  <si>
-    <t>newsletter</t>
-  </si>
-  <si>
-    <t>mail</t>
-  </si>
-  <si>
-    <t>identifiant abonné</t>
-  </si>
-  <si>
-    <t>mail abonné</t>
-  </si>
-  <si>
-    <t>prestation</t>
-  </si>
-  <si>
-    <t>tarif</t>
-  </si>
-  <si>
     <t>FLOAT</t>
   </si>
   <si>
@@ -225,27 +156,12 @@
     <t>nom de la prestation</t>
   </si>
   <si>
-    <t>slider</t>
-  </si>
-  <si>
-    <t>bg_image</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
     <t xml:space="preserve"> identifiant du slide</t>
   </si>
   <si>
-    <t>texte dans la bannière</t>
-  </si>
-  <si>
     <t>source  de l'image de fond du slide</t>
   </si>
   <si>
-    <t>profil</t>
-  </si>
-  <si>
     <t>description du profil (ex: admin, utilisateur,ect..)</t>
   </si>
   <si>
@@ -255,18 +171,6 @@
     <t>libellé du profil</t>
   </si>
   <si>
-    <t>role</t>
-  </si>
-  <si>
-    <t>identifiant du role</t>
-  </si>
-  <si>
-    <t>libellé du role</t>
-  </si>
-  <si>
-    <t>description du role</t>
-  </si>
-  <si>
     <t>Catégories</t>
   </si>
   <si>
@@ -322,13 +226,235 @@
   </si>
   <si>
     <t>#profil_id</t>
+  </si>
+  <si>
+    <t>profil_id</t>
+  </si>
+  <si>
+    <t>profil_libelle</t>
+  </si>
+  <si>
+    <t>profil_description</t>
+  </si>
+  <si>
+    <t>Utilisateurs</t>
+  </si>
+  <si>
+    <t>Profils</t>
+  </si>
+  <si>
+    <t>Permission du profil</t>
+  </si>
+  <si>
+    <t>#permission_id</t>
+  </si>
+  <si>
+    <t>identifiant de la permission</t>
+  </si>
+  <si>
+    <t>libellé de la permission</t>
+  </si>
+  <si>
+    <t>description de la permission</t>
+  </si>
+  <si>
+    <t>Permission</t>
+  </si>
+  <si>
+    <t>permission_id</t>
+  </si>
+  <si>
+    <t>permission_libelle</t>
+  </si>
+  <si>
+    <t>permission_description</t>
+  </si>
+  <si>
+    <t>Galerie d'image</t>
+  </si>
+  <si>
+    <t>img_id</t>
+  </si>
+  <si>
+    <t>img_libelle</t>
+  </si>
+  <si>
+    <t>img_slug</t>
+  </si>
+  <si>
+    <t>img_src</t>
+  </si>
+  <si>
+    <t>img_description</t>
+  </si>
+  <si>
+    <t>img_auteur</t>
+  </si>
+  <si>
+    <t>img_date_publi</t>
+  </si>
+  <si>
+    <t>img_validation</t>
+  </si>
+  <si>
+    <t>BOOLEAN</t>
+  </si>
+  <si>
+    <t>validation par le modérateur</t>
+  </si>
+  <si>
+    <t>Commentaire d'image</t>
+  </si>
+  <si>
+    <t>comment_id</t>
+  </si>
+  <si>
+    <t>identifiant du commentaire</t>
+  </si>
+  <si>
+    <t>comment_date</t>
+  </si>
+  <si>
+    <t>date de la dernière modification</t>
+  </si>
+  <si>
+    <t>comment_last_date</t>
+  </si>
+  <si>
+    <t>date de publication du commentaire</t>
+  </si>
+  <si>
+    <t>comment_content</t>
+  </si>
+  <si>
+    <t>cotenu du commentaire</t>
+  </si>
+  <si>
+    <t>#user_id</t>
+  </si>
+  <si>
+    <t>#img_id</t>
+  </si>
+  <si>
+    <t>Evenement</t>
+  </si>
+  <si>
+    <t>event_id</t>
+  </si>
+  <si>
+    <t>event_name</t>
+  </si>
+  <si>
+    <t>event_slug</t>
+  </si>
+  <si>
+    <t>event_img</t>
+  </si>
+  <si>
+    <t>event_content</t>
+  </si>
+  <si>
+    <t>event_create_date</t>
+  </si>
+  <si>
+    <t>event_start_date</t>
+  </si>
+  <si>
+    <t>event_end_date</t>
+  </si>
+  <si>
+    <t>event_capacity</t>
+  </si>
+  <si>
+    <t>date de publication de l'événement</t>
+  </si>
+  <si>
+    <t>Abonnées Newsletter</t>
+  </si>
+  <si>
+    <t>Prestations</t>
+  </si>
+  <si>
+    <t>prestation_id</t>
+  </si>
+  <si>
+    <t>prestation_name</t>
+  </si>
+  <si>
+    <t>prestation_slug</t>
+  </si>
+  <si>
+    <t>prestation_description</t>
+  </si>
+  <si>
+    <t>prestation_tarif</t>
+  </si>
+  <si>
+    <t>categorie_id</t>
+  </si>
+  <si>
+    <t>categorie_slug</t>
+  </si>
+  <si>
+    <t>categorie_name</t>
+  </si>
+  <si>
+    <t>categorie_description</t>
+  </si>
+  <si>
+    <t>Slider</t>
+  </si>
+  <si>
+    <t>slide_id</t>
+  </si>
+  <si>
+    <t>slide_bg_image</t>
+  </si>
+  <si>
+    <t>slide_banner_content</t>
+  </si>
+  <si>
+    <t>contenu dans la bannière</t>
+  </si>
+  <si>
+    <t>identifiant abonné de la newsletter</t>
+  </si>
+  <si>
+    <t>mail abonné de la newsletter</t>
+  </si>
+  <si>
+    <t>Newsletter</t>
+  </si>
+  <si>
+    <t>subscriber_id</t>
+  </si>
+  <si>
+    <t>subscreiber_email</t>
+  </si>
+  <si>
+    <t>newsletter_id</t>
+  </si>
+  <si>
+    <t>newsletter_libelle</t>
+  </si>
+  <si>
+    <t>newsletter_content</t>
+  </si>
+  <si>
+    <t>contenu de la newsletter</t>
+  </si>
+  <si>
+    <t>nom de la newsletter</t>
+  </si>
+  <si>
+    <t>identifiant de la newsletter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -353,9 +479,34 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -381,7 +532,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -395,12 +546,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
+      <font>
+        <b/>
+      </font>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -432,9 +595,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EF723056-E4B8-4061-80B1-0C4921BF2AB7}" name="Tableau2" displayName="Tableau2" ref="A1:C1048575" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A1:C1048575" xr:uid="{369D7CF8-C4A2-4986-BDE3-A03DA8D931CC}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{94063425-DECB-4A76-A3E0-1A81E0A5F2CB}" name="Nom du champ" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{94063425-DECB-4A76-A3E0-1A81E0A5F2CB}" name="Nom du champ" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{019612D5-0932-47FE-B3F8-53219A6E2896}" name="Type de données" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{066C183E-2CB4-4A03-95ED-B26B08FA63FF}" name="Intitulé du champ" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{066C183E-2CB4-4A03-95ED-B26B08FA63FF}" name="Intitulé du champ" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -740,22 +903,22 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" style="2" customWidth="1"/>
     <col min="2" max="2" width="20.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="43.5703125" style="1" customWidth="1"/>
     <col min="4" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -766,576 +929,725 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B5" s="1" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>94</v>
+      <c r="A11" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>95</v>
+      <c r="A12" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>96</v>
+      <c r="A13" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>72</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="1" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="1" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C29" s="1" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>9</v>
+      <c r="A33" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>40</v>
+      <c r="A34" s="6" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>52</v>
+        <v>91</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>3</v>
+      <c r="A36" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>45</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>44</v>
+      <c r="A37" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>46</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>13</v>
+      <c r="A38" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>47</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>41</v>
+      <c r="A39" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>11</v>
+      <c r="A40" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>53</v>
+        <v>103</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>3</v>
+      <c r="A44" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>54</v>
+      <c r="A45" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>57</v>
+        <v>106</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>3</v>
+      <c r="A47" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>60</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>4</v>
+      <c r="A48" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>13</v>
+      <c r="A49" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>85</v>
+        <v>27</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>84</v>
+      <c r="A50" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>61</v>
+      <c r="A51" s="6" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>58</v>
+      <c r="A52" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>62</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>78</v>
+        <v>132</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>79</v>
+      <c r="A54" s="6" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>13</v>
+      <c r="A55" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>80</v>
+        <v>138</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>4</v>
+      <c r="A56" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>81</v>
+        <v>137</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>11</v>
+      <c r="A57" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>82</v>
+        <v>136</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>64</v>
+      <c r="A58" s="6" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>3</v>
+      <c r="A59" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>65</v>
+      <c r="A60" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>66</v>
+      <c r="A61" s="2" t="s">
+        <v>116</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>68</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>